<commit_message>
partial update import asset
</commit_message>
<xml_diff>
--- a/public/templates/asset-import.xlsx
+++ b/public/templates/asset-import.xlsx
@@ -8,7 +8,8 @@
     <sheet sheetId="3" name="Project ID" r:id="rId3"/>
     <sheet sheetId="4" name="Site ID" r:id="rId4"/>
     <sheet sheetId="5" name="Asset Model ID" r:id="rId5"/>
-    <sheet sheetId="6" name="Component ID" r:id="rId6"/>
+    <sheet sheetId="6" name="Asset Class ID" r:id="rId6"/>
+    <sheet sheetId="7" name="Component ID" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -19,14 +20,8 @@
     <numFmt formatCode="yyyy/mm/dd" numFmtId="100"/>
     <numFmt formatCode="yyyy/mm/dd hh:mm:ss" numFmtId="101"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
-      <name val="Arial"/>
-      <sz val="11"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
       <name val="Arial"/>
       <sz val="11"/>
       <family val="1"/>
@@ -73,12 +68,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -95,145 +89,189 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showRuler="1" showWhiteSpace="0" showZeros="1" tabSelected="0" windowProtection="0" showOutlineSymbols="1" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0" workbookViewId="0" zoomScale="100"/>
+    <sheetView defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showRuler="1" showWhiteSpace="0" showZeros="1" tabSelected="0" windowProtection="0" showOutlineSymbols="1" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0" workbookViewId="0" zoomScale="100">
+      <pane state="frozen" topLeftCell="A2" xSplit="0" ySplit="1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col width="21.45" min="1" max="1" bestFit="1" customWidth="1"/>
-    <col width="21.45" min="2" max="2" bestFit="1" customWidth="1"/>
-    <col width="16.5" min="3" max="3" bestFit="1" customWidth="1"/>
-    <col width="28.049999999999997" min="4" max="4" bestFit="1" customWidth="1"/>
+    <col width="24.75" min="1" max="1" bestFit="1" customWidth="1"/>
+    <col width="24.75" min="2" max="2" bestFit="1" customWidth="1"/>
+    <col width="19.799999999999997" min="3" max="3" bestFit="1" customWidth="1"/>
+    <col width="31.349999999999998" min="4" max="4" bestFit="1" customWidth="1"/>
     <col width="28.049999999999997" min="5" max="5" bestFit="1" customWidth="1"/>
     <col width="19.799999999999997" min="6" max="6" bestFit="1" customWidth="1"/>
-    <col width="39.599999999999994" min="7" max="7" bestFit="1" customWidth="1"/>
-    <col width="26.4" min="8" max="8" bestFit="1" customWidth="1"/>
-    <col width="23.099999999999998" min="9" max="9" bestFit="1" customWidth="1"/>
-    <col width="14.85" min="10" max="10" bestFit="1" customWidth="1"/>
-    <col width="21.45" min="11" max="11" bestFit="1" customWidth="1"/>
-    <col width="23.099999999999998" min="12" max="12" bestFit="1" customWidth="1"/>
-    <col width="26.4" min="13" max="13" bestFit="1" customWidth="1"/>
-    <col width="23.099999999999998" min="14" max="14" bestFit="1" customWidth="1"/>
+    <col width="26.4" min="7" max="7" bestFit="1" customWidth="1"/>
+    <col width="23.099999999999998" min="8" max="8" bestFit="1" customWidth="1"/>
+    <col width="14.85" min="9" max="9" bestFit="1" customWidth="1"/>
+    <col width="21.45" min="10" max="10" bestFit="1" customWidth="1"/>
+    <col width="23.099999999999998" min="11" max="11" bestFit="1" customWidth="1"/>
+    <col width="26.4" min="12" max="12" bestFit="1" customWidth="1"/>
+    <col width="23.099999999999998" min="13" max="13" bestFit="1" customWidth="1"/>
+    <col width="18.15" min="14" max="14" bestFit="1" customWidth="1"/>
     <col width="18.15" min="15" max="15" bestFit="1" customWidth="1"/>
     <col width="28.049999999999997" min="16" max="16" bestFit="1" customWidth="1"/>
-    <col width="24.75" min="17" max="17" bestFit="1" customWidth="1"/>
-    <col width="19.799999999999997" min="18" max="18" bestFit="1" customWidth="1"/>
-    <col width="21.45" min="19" max="19" bestFit="1" customWidth="1"/>
-    <col width="29.7" min="20" max="20" bestFit="1" customWidth="1"/>
-    <col width="14.85" min="21" max="21" bestFit="1" customWidth="1"/>
-    <col width="19.799999999999997" min="22" max="22" bestFit="1" customWidth="1"/>
+    <col width="28.049999999999997" min="17" max="17" bestFit="1" customWidth="1"/>
+    <col width="24.75" min="18" max="18" bestFit="1" customWidth="1"/>
+    <col width="24.75" min="19" max="19" bestFit="1" customWidth="1"/>
+    <col width="19.799999999999997" min="20" max="20" bestFit="1" customWidth="1"/>
+    <col width="19.799999999999997" min="21" max="21" bestFit="1" customWidth="1"/>
+    <col width="21.45" min="22" max="22" bestFit="1" customWidth="1"/>
+    <col width="21.45" min="23" max="23" bestFit="1" customWidth="1"/>
+    <col width="29.7" min="24" max="24" bestFit="1" customWidth="1"/>
+    <col width="29.7" min="25" max="25" bestFit="1" customWidth="1"/>
+    <col width="14.85" min="26" max="26" bestFit="1" customWidth="1"/>
+    <col width="14.85" min="27" max="27" bestFit="1" customWidth="1"/>
+    <col width="19.799999999999997" min="28" max="28" bestFit="1" customWidth="1"/>
+    <col width="19.799999999999997" min="29" max="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Tagging id</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Project id</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>Site id</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>Asset model id</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Tagging id *</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Project id *</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Site id *</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Asset model id *</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Asset class id</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>DO number</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>Warranty expired date</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Computer name</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>IP computer</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>Computer IP</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>CPU sn</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Monitor sn</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>Keyboard sn</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>Shipping date</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>Mouse id</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>Mouse sn</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>Floopy disk id</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>Floopy disk sn</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>Processor id</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>Processor sn</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>Memory id</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>Memory sn</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
         <is>
           <t>Hardisk id</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>Hardisk sn</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
         <is>
           <t>CD / DVD rom id</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
+        <is>
+          <t>CD / DVD rom sn</t>
+        </is>
+      </c>
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>NIC id</t>
         </is>
       </c>
-      <c r="V1" s="4" t="inlineStr">
+      <c r="AA1" s="3" t="inlineStr">
+        <is>
+          <t>NIC sn</t>
+        </is>
+      </c>
+      <c r="AB1" s="3" t="inlineStr">
         <is>
           <t>Others id</t>
+        </is>
+      </c>
+      <c r="AC1" s="3" t="inlineStr">
+        <is>
+          <t>Others sn</t>
         </is>
       </c>
     </row>
@@ -251,17 +289,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showRuler="1" showWhiteSpace="0" showZeros="1" tabSelected="0" windowProtection="0" showOutlineSymbols="1" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0" workbookViewId="0" zoomScale="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col width="196.9" min="1" max="1" bestFit="1" customWidth="1"/>
+    <col width="199.10000000000002" min="1" max="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Panduan upload</t>
         </is>
@@ -270,28 +308,35 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>1. Tagging id harus diisi dan unik (tidak boleh sama)</t>
+          <t>1. Lengkapi semua data-data yang ada pada sheet Upload</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>2. Row Project id, Site id, Asset model id, Asset class id diisi dengan id masing-masing. Id bisa dicek pada masing-masing sheet sesuai nama row</t>
+          <t>2. Kolom pada sheet Upload dengan simbol (*) artinya wajib diisi</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>3. Row Project id, Site id, Asset model id wajib diisi</t>
+          <t>3. Tagging id harus unik (tidak boleh sama)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>4. Row Mouse id, Floopy disk id, Processor id, Memory id, Hardisk id, CD / DVD room id, NIC id, Other id diisi dengan id masing-masing. Id bisa dicek pada sheet `Components ID`</t>
+          <t>4. Kolom Project id, Site id, Asset model id, Asset class id diisi dengan id masing-masing. Id bisa dicek pada masing-masing sheet sesuai nama kolom</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>5. Kolom Mouse id, Floopy disk id, Processor id, Memory id, Hardisk id, CD / DVD room id, NIC id, Other id diisi dengan id masing-masing. Id bisa dicek pada sheet `Components ID`</t>
         </is>
       </c>
     </row>
@@ -320,12 +365,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Project id</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
@@ -428,12 +473,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Site id</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
@@ -3908,12 +3953,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Asset model id</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
@@ -9817,6 +9862,160 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showRowColHeaders="1" showRuler="1" showWhiteSpace="0" showZeros="1" tabSelected="0" windowProtection="0" showOutlineSymbols="1" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0" workbookViewId="0" zoomScale="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <cols>
+    <col width="28.049999999999997" min="1" max="1" bestFit="1" customWidth="1"/>
+    <col width="30.800000000000004" min="2" max="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Asset class id</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>NBADVUSR</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Notebook Advance User</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>NBADVUSR2</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Notebook Advance User 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>NBPERFUSR</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Notebook Performance User</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>NBREGUSR</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Notebook Reg. User</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>NBREGUSR2</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Notebook Reg. User 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>PERFPC</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Performance PC</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>PERFPC1</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>Performance PC 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="inlineStr">
+        <is>
+          <t>PERFPC2</t>
+        </is>
+      </c>
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Performance PC 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="inlineStr">
+        <is>
+          <t>STDPC1</t>
+        </is>
+      </c>
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>Standard PC 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>safety net</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <printOptions gridLines="0" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins left="0.75" right="0.75" top="1.0" bottom="1.0" header="0.5" footer="0.5"/>
+  <pageSetup/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
@@ -9833,17 +10032,17 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Component id</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Component type</t>
         </is>

</xml_diff>